<commit_message>
Renaming the file name
</commit_message>
<xml_diff>
--- a/Week 7- TIme Sheet/Timesheet.xlsx
+++ b/Week 7- TIme Sheet/Timesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4e69d9f31af72fd/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patha\OneDrive\Documents\My-salon\Week 7- TIme Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{FCBBA73B-8C29-4AC8-894C-0CB43DB2DD4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BAB25F9D-44A2-4C84-8CAE-275C175E4AB8}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{FCBBA73B-8C29-4AC8-894C-0CB43DB2DD4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F0AAD576-8C4D-4091-99FE-F0EAD50B583F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F1D8994-60BF-442A-BCE4-58B7C1EAEC30}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Hour 1</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Work Division for next Week</t>
+  </si>
+  <si>
+    <t>Hour 14</t>
+  </si>
+  <si>
+    <t>Working on Assignment 2</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2018F03-1563-459D-BD51-FA785D6E9CA4}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +581,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>